<commit_message>
add fuse to PCB, update BOM and garbers
</commit_message>
<xml_diff>
--- a/PCBs/PCB_Luciernagas/Project Outputs for PCB_Luciernagas/BOM_PCB_Luciernagas.xlsx
+++ b/PCBs/PCB_Luciernagas/Project Outputs for PCB_Luciernagas/BOM_PCB_Luciernagas.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B4D28A0-116F-4B86-AC34-B8811D991B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{14B800EF-8C23-4842-8CF5-CE5E9303597E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" xr2:uid="{A4C5067D-B133-464D-906F-CDEB19B41193}"/>
+    <workbookView xWindow="4245" yWindow="4245" windowWidth="21600" windowHeight="11835" xr2:uid="{DE4ACD22-8180-4220-8B6B-779212CBB989}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PCB_Luciernagas" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="63">
   <si>
     <t>Comment</t>
   </si>
@@ -105,6 +105,15 @@
     <t>D11, D12</t>
   </si>
   <si>
+    <t>1206L200</t>
+  </si>
+  <si>
+    <t>Resettable Fuse</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
     <t>ATMEGA328PB-AN</t>
   </si>
   <si>
@@ -141,7 +150,7 @@
     <t>LED</t>
   </si>
   <si>
-    <t>LED1</t>
+    <t>LED CHG</t>
   </si>
   <si>
     <t>DMP3125L-7</t>
@@ -613,8 +622,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB94E4E-0D18-4497-9D38-E63C722F7D74}">
-  <dimension ref="A1:D23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{511A4645-FEEA-4310-9A86-F5E0CE34263B}">
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -770,10 +779,10 @@
         <v>27</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D11" s="3">
         <v>1</v>
@@ -781,13 +790,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12" s="3">
         <v>1</v>
@@ -795,10 +804,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>33</v>
@@ -832,7 +841,7 @@
         <v>39</v>
       </c>
       <c r="D15" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -854,63 +863,63 @@
         <v>43</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D17" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D18" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D19" s="3">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D20" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>53</v>
@@ -944,6 +953,20 @@
         <v>59</v>
       </c>
       <c r="D23" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>